<commit_message>
Updating Asset Swap Example Workbook - Adding Bloomberg Screenshots
</commit_message>
<xml_diff>
--- a/10 Asset Swap Pricing Examples/AssetSwapPricingExamples.xlsx
+++ b/10 Asset Swap Pricing Examples/AssetSwapPricingExamples.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\BOOK\.SWAPS_BOOK\10 Asset Swap Pricing Examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52FE9EB2-DAC7-4919-9C54-E99FD6933E17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6E65EF7-F784-4065-8BCB-52C1781ACB80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{04F0DFD9-E694-4A57-B6D9-D4AB214DD37F}"/>
+    <workbookView xWindow="3075" yWindow="3075" windowWidth="38700" windowHeight="15345" activeTab="1" xr2:uid="{04F0DFD9-E694-4A57-B6D9-D4AB214DD37F}"/>
   </bookViews>
   <sheets>
     <sheet name="Yield-Yield Spread" sheetId="1" r:id="rId1"/>
     <sheet name="Par-Par Spread" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029" calcOnSave="0" concurrentCalc="0"/>
+  <calcPr calcId="191029" calcCompleted="0" calcOnSave="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -208,14 +208,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>381001</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>600076</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>22860</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>297181</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>192406</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>180467</xdr:rowOff>
     </xdr:to>
@@ -240,8 +240,184 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="990601" y="434340"/>
-          <a:ext cx="4518660" cy="340487"/>
+          <a:off x="600076" y="508635"/>
+          <a:ext cx="4450080" cy="348107"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>95251</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>100534</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{758BB827-D6BB-1791-7E9F-F163CCA9F5CF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5391150" y="95251"/>
+          <a:ext cx="4981575" cy="3539058"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>152399</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>62780</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32390FAA-63FE-9D72-E510-5BCD74777F77}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5400675" y="3876674"/>
+          <a:ext cx="5029200" cy="4482381"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>139492</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>57149</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A070D373-AA0D-6390-FF28-F83EF069D5CE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10972800" y="1387267"/>
+          <a:ext cx="6315075" cy="2203657"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>267579</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>86107</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ABD00ED2-A3BF-9A79-F68F-94C2AF663A94}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11020425" y="5648325"/>
+          <a:ext cx="6296904" cy="2734057"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -291,6 +467,94 @@
         <a:xfrm>
           <a:off x="708660" y="609600"/>
           <a:ext cx="3246120" cy="752538"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>220291</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>105512</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{47E15BB7-EC23-F9A1-472B-06DCB0C1F9FF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4438650" y="5791200"/>
+          <a:ext cx="8716591" cy="5277587"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>210761</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>750</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{07F64527-6FD9-1736-B540-5A0831A373CC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4467225" y="66675"/>
+          <a:ext cx="8678486" cy="5372850"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -599,132 +863,86 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6508515-2C24-4582-9380-E99C21EB9331}">
-  <dimension ref="B2:G17"/>
+  <dimension ref="B2:C32"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.77734375" customWidth="1"/>
-    <col min="6" max="6" width="15.77734375" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" customWidth="1"/>
+    <col min="6" max="6" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B2" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>1</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F8" t="s">
-        <v>1</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>3</v>
       </c>
       <c r="C9" s="3">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="F9" t="s">
-        <v>3</v>
-      </c>
-      <c r="G9" s="3">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>4</v>
       </c>
       <c r="C10" s="2">
         <v>2026</v>
       </c>
-      <c r="F10" t="s">
-        <v>4</v>
-      </c>
-      <c r="G10" s="2">
-        <v>2026</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>13</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F11" t="s">
-        <v>13</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>5</v>
       </c>
       <c r="C12" s="8">
         <v>99.02</v>
       </c>
-      <c r="F12" t="s">
-        <v>5</v>
-      </c>
-      <c r="G12" s="8">
-        <v>65.397999999999996</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>6</v>
       </c>
       <c r="C13" s="4">
         <v>6.4000000000000003E-3</v>
       </c>
-      <c r="F13" t="s">
-        <v>6</v>
-      </c>
-      <c r="G13" s="4">
-        <v>9.1880000000000003E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C14" s="2"/>
-      <c r="G14" s="2"/>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>7</v>
       </c>
       <c r="C15" s="4">
         <v>9.1999999999999998E-3</v>
       </c>
-      <c r="F15" t="s">
-        <v>7</v>
-      </c>
-      <c r="G15" s="4">
-        <v>9.1999999999999998E-3</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>8</v>
       </c>
@@ -732,15 +950,8 @@
         <f>C13-C15</f>
         <v>-2.7999999999999995E-3</v>
       </c>
-      <c r="F16" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G16" s="5">
-        <f>G13-G15</f>
-        <v>8.2680000000000003E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>11</v>
       </c>
@@ -748,11 +959,86 @@
         <f>C16*10000</f>
         <v>-27.999999999999996</v>
       </c>
-      <c r="F17" t="s">
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" s="3">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="2">
+        <v>2026</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" s="8">
+        <v>65.397999999999996</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" s="4">
+        <v>9.1880000000000003E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C29" s="2"/>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30" s="4">
+        <v>9.1999999999999998E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B31" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31" s="5">
+        <f>C28-C30</f>
+        <v>8.2680000000000003E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
         <v>11</v>
       </c>
-      <c r="G17" s="6">
-        <f>G16*10000</f>
+      <c r="C32" s="6">
+        <f>C31*10000</f>
         <v>826.80000000000007</v>
       </c>
     </row>
@@ -764,157 +1050,101 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52ED2D0F-45FF-4830-9332-6222390A0C05}">
-  <dimension ref="B2:G28"/>
+  <dimension ref="B2:C47"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="20.77734375" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.77734375" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" customWidth="1"/>
+    <col min="16" max="16" width="35.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B2" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>1</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F10" t="s">
-        <v>1</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>3</v>
       </c>
       <c r="C11" s="3">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="F11" t="s">
-        <v>3</v>
-      </c>
-      <c r="G11" s="3">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>4</v>
       </c>
       <c r="C12" s="2">
         <v>2026</v>
       </c>
-      <c r="F12" t="s">
-        <v>4</v>
-      </c>
-      <c r="G12" s="2">
-        <v>2026</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>13</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F13" t="s">
-        <v>13</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>5</v>
       </c>
       <c r="C14" s="8">
         <v>104.58</v>
       </c>
-      <c r="F14" t="s">
-        <v>5</v>
-      </c>
-      <c r="G14" s="8">
-        <v>75.28</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>6</v>
       </c>
       <c r="C15" s="4">
         <v>6.4000000000000003E-3</v>
       </c>
-      <c r="F15" t="s">
-        <v>6</v>
-      </c>
-      <c r="G15" s="4">
-        <v>4.58E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>7</v>
       </c>
       <c r="C17" s="4">
         <v>4.4000000000000003E-3</v>
       </c>
-      <c r="F17" t="s">
-        <v>7</v>
-      </c>
-      <c r="G17" s="4">
-        <v>4.4000000000000003E-3</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>16</v>
       </c>
       <c r="C18" s="6">
         <v>10</v>
       </c>
-      <c r="F18" t="s">
-        <v>16</v>
-      </c>
-      <c r="G18" s="6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>17</v>
       </c>
       <c r="C19" s="6">
         <v>10</v>
       </c>
-      <c r="F19" t="s">
-        <v>17</v>
-      </c>
-      <c r="G19" s="6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
         <v>18</v>
       </c>
@@ -922,15 +1152,8 @@
         <f>((C11-C17)*C18+(100-C14)/100)/C19</f>
         <v>-3.9799999999999983E-3</v>
       </c>
-      <c r="F21" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G21" s="5">
-        <f>((G11-G17)*G18+(100-G14)/100)/G19</f>
-        <v>5.0319999999999997E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>11</v>
       </c>
@@ -938,15 +1161,8 @@
         <f>C21*10000</f>
         <v>-39.799999999999983</v>
       </c>
-      <c r="F22" t="s">
-        <v>11</v>
-      </c>
-      <c r="G22" s="10">
-        <f>G21*10000</f>
-        <v>503.2</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>19</v>
       </c>
@@ -954,15 +1170,8 @@
         <f>(C11-C17)*C18</f>
         <v>5.9999999999999984E-3</v>
       </c>
-      <c r="F24" t="s">
-        <v>19</v>
-      </c>
-      <c r="G24" s="4">
-        <f>(G11-G17)*G18</f>
-        <v>0.25600000000000001</v>
-      </c>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>20</v>
       </c>
@@ -970,15 +1179,8 @@
         <f>(100-C14)/100</f>
         <v>-4.579999999999998E-2</v>
       </c>
-      <c r="F25" t="s">
-        <v>20</v>
-      </c>
-      <c r="G25" s="4">
-        <f>(100-G14)/100</f>
-        <v>0.24719999999999998</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>21</v>
       </c>
@@ -986,16 +1188,131 @@
         <f>(C24+C25)/C19</f>
         <v>-3.9799999999999983E-3</v>
       </c>
-      <c r="F26" t="s">
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C28" s="9"/>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B30" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>1</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>3</v>
+      </c>
+      <c r="C32" s="3">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>4</v>
+      </c>
+      <c r="C33" s="2">
+        <v>2026</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>13</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>5</v>
+      </c>
+      <c r="C35" s="8">
+        <v>75.28</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>6</v>
+      </c>
+      <c r="C36" s="4">
+        <v>4.58E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>7</v>
+      </c>
+      <c r="C38" s="4">
+        <v>4.4000000000000003E-3</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>16</v>
+      </c>
+      <c r="C39" s="6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>17</v>
+      </c>
+      <c r="C40" s="6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B42" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C42" s="5">
+        <f>((C32-C38)*C39+(100-C35)/100)/C40</f>
+        <v>5.0319999999999997E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>11</v>
+      </c>
+      <c r="C43" s="10">
+        <f>C42*10000</f>
+        <v>503.2</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>19</v>
+      </c>
+      <c r="C45" s="4">
+        <f>(C32-C38)*C39</f>
+        <v>0.25600000000000001</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>20</v>
+      </c>
+      <c r="C46" s="4">
+        <f>(100-C35)/100</f>
+        <v>0.24719999999999998</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
         <v>21</v>
       </c>
-      <c r="G26" s="11">
-        <f>(G24+G25)/G19</f>
+      <c r="C47" s="11">
+        <f>(C45+C46)/C40</f>
         <v>5.0319999999999997E-2</v>
       </c>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C28" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>